<commit_message>
DATE : 19th may 2022
</commit_message>
<xml_diff>
--- a/DSA Sheet by Arsh (45 Days Plan).xlsx
+++ b/DSA Sheet by Arsh (45 Days Plan).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf10ee88a5560afd/Desktop/^Ncrackyourinternship/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{3D0027D1-9864-4A06-BC74-E79705549ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{452B5F66-9E12-4D61-B7BD-F473BD5F45DE}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3D0027D1-9864-4A06-BC74-E79705549ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{103F2AD2-3C18-439B-AFB3-560B8934143A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="327">
   <si>
     <t>Status</t>
   </si>
@@ -1582,8 +1582,8 @@
   <dimension ref="A1:H339"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="32.1" customHeight="1"/>
@@ -2602,6 +2602,9 @@
       <c r="B99" s="28" t="s">
         <v>325</v>
       </c>
+      <c r="C99" s="20" t="s">
+        <v>321</v>
+      </c>
       <c r="F99" s="1" t="s">
         <v>6</v>
       </c>
@@ -2627,6 +2630,9 @@
       <c r="B101" s="22" t="s">
         <v>98</v>
       </c>
+      <c r="C101" s="20" t="s">
+        <v>321</v>
+      </c>
       <c r="D101" s="1" t="s">
         <v>6</v>
       </c>
@@ -2733,9 +2739,6 @@
       <c r="B109" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="C109" s="20" t="s">
-        <v>321</v>
-      </c>
       <c r="D109" s="1" t="s">
         <v>6</v>
       </c>
@@ -2762,6 +2765,9 @@
       </c>
       <c r="B112" s="22" t="s">
         <v>108</v>
+      </c>
+      <c r="C112" s="20" t="s">
+        <v>321</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>6</v>

</xml_diff>